<commit_message>
fix: excel file edited
</commit_message>
<xml_diff>
--- a/data/employee_list.xlsx
+++ b/data/employee_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad6921c7f953aa9b/Desktop/New folder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\JavaScript Projects\leave-management-system\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_37607AECFD7D783525BC9084D90ACB8EAB499A99" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793E4808-7BA0-4BCA-8E3B-9EB11077D9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2010" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2959,7 +2959,7 @@
   <dimension ref="A1:G256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3013,7 +3013,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="7">
-        <v>9958024468</v>
+        <v>8145312848</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
fix: excel files updated
</commit_message>
<xml_diff>
--- a/data/employee_list.xlsx
+++ b/data/employee_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\JavaScript Projects\leave-management-system\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad6921c7f953aa9b/Desktop/New folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793E4808-7BA0-4BCA-8E3B-9EB11077D9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_37607AECFD7D783525BC9084D90ACB8EAB499A99" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="2010" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2959,7 +2959,7 @@
   <dimension ref="A1:G256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3013,7 +3013,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="7">
-        <v>8145312848</v>
+        <v>9958024468</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>12</v>

</xml_diff>